<commit_message>
new runsettings, testing CT5 examples, working
</commit_message>
<xml_diff>
--- a/data/exp_raw/exptables.xlsx
+++ b/data/exp_raw/exptables.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blomerusjm\.julia\environments\WatVal\LifeVal\data\exp_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2573E9-8D74-4584-94CC-5475EA963B42}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{857C3288-00D9-4C59-99CC-B6200E546659}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9A471A6D-0FC7-472A-9A37-059D26A05113}"/>
+    <workbookView xWindow="9460" yWindow="890" windowWidth="8780" windowHeight="9850" activeTab="5" xr2:uid="{9A471A6D-0FC7-472A-9A37-059D26A05113}"/>
   </bookViews>
   <sheets>
-    <sheet name="ufs1" sheetId="3" r:id="rId1"/>
-    <sheet name="ASSA" sheetId="4" r:id="rId2"/>
-    <sheet name="ul1" sheetId="5" r:id="rId3"/>
-    <sheet name="ulp" sheetId="6" r:id="rId4"/>
+    <sheet name="zero" sheetId="7" r:id="rId1"/>
+    <sheet name="ufs1" sheetId="3" r:id="rId2"/>
+    <sheet name="ASSA" sheetId="4" r:id="rId3"/>
+    <sheet name="ul1" sheetId="5" r:id="rId4"/>
+    <sheet name="ulp" sheetId="6" r:id="rId5"/>
+    <sheet name="ea1" sheetId="8" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="MORT_SENS">#REF!</definedName>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="9">
   <si>
     <t>SPCODE</t>
   </si>
@@ -482,10 +484,211 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E526C135-9A81-49F6-8FF3-3081AE0851C7}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9F2689-05EE-40EC-9F38-99BDBE68D21B}">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -682,7 +885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83514799-2DCE-48ED-BF8E-762E953555C1}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -766,7 +969,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CEB23C7-CDC6-457A-A862-8B1283D72D7F}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -850,7 +1053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92E01C65-D766-468C-846C-EB924F6ADCFA}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -932,4 +1135,206 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF275B10-8FE7-4C1A-8202-3BB397D48B70}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>325</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>75/12</f>
+        <v>6.25</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <v>150</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0.03</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>